<commit_message>
Implemented multithreading. Result is still too low.
</commit_message>
<xml_diff>
--- a/examples.xlsx
+++ b/examples.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kylian\Documents\Programming\C\OptionPricingMonteCarlo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8718C738-91DE-4179-82EF-9FAA4EF8F36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BF4DC2-E420-458D-BF8C-99030FD54F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="21840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asset 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t xml:space="preserve">Name: </t>
   </si>
@@ -116,6 +117,12 @@
   </si>
   <si>
     <t>2.76???</t>
+  </si>
+  <si>
+    <t>PARAMS:</t>
+  </si>
+  <si>
+    <t>MOCKED_RANDOM_NUMBERS:</t>
   </si>
 </sst>
 </file>
@@ -444,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,4 +631,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C689EB-F515-422C-B30D-9D6104C8421D}">
+  <dimension ref="B2:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.9</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0.8</v>
+      </c>
+      <c r="J3">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>